<commit_message>
update the evaluation outputs
</commit_message>
<xml_diff>
--- a/Class PBH.xlsx
+++ b/Class PBH.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johncarroll/Projects/pfg-product-categorization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46B805FE-B65E-BE41-9EF5-DAB55595A6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381CF1BE-7015-154B-BFAD-2C2D823BB004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="3640" windowWidth="18200" windowHeight="18440" xr2:uid="{C0CAB85E-6C73-3D47-ABF4-8B6291248F80}"/>
+    <workbookView xWindow="5860" yWindow="2780" windowWidth="29660" windowHeight="17980" xr2:uid="{C0CAB85E-6C73-3D47-ABF4-8B6291248F80}"/>
   </bookViews>
   <sheets>
-    <sheet name="EasyClassPBHview" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="EasyClassPBHview" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="4" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="157">
   <si>
     <t>Row Labels</t>
   </si>
@@ -504,16 +508,37 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Class_Name</t>
+  </si>
+  <si>
+    <t>PBH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -527,7 +552,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -535,17 +560,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF44B3E1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1729,7 +1770,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA4D91C7-4D39-7D47-9188-FF492C443C20}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AA4D91C7-4D39-7D47-9188-FF492C443C20}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A158" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -2702,727 +2743,2145 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0467E58A-B74D-FD42-9A1F-675A11B32646}">
+  <dimension ref="A1:B140"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="286" workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{0467E58A-B74D-FD42-9A1F-675A11B32646}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F15A83A4-A21B-B047-AB53-9E06A0133856}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A3:A158"/>
+  <dimension ref="A3:D158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="169" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A135" zoomScale="169" workbookViewId="0">
+      <selection activeCell="C148" sqref="C3:D148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C7" s="5"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C8" s="5"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C13" s="5"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C17" s="5"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C18" s="5"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C19" s="5"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C22" s="5"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C24" s="5"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C26" s="5"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C27" s="5"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C28" s="5"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C29" s="5"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C30" s="5"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C32" s="5"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C33" s="5"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C34" s="5"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C35" s="5"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C36" s="5"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C37" s="5"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C38" s="5"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C39" s="5"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C40" s="5"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C41" s="5"/>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C42" s="5"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C43" s="5"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C44" s="5"/>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C45" s="5"/>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C46" s="5"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C47" s="5"/>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C48" s="5"/>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C49" s="5"/>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C50" s="5"/>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C51" s="5"/>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C52" s="5"/>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C53" s="5"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C54" s="5"/>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C55" s="5"/>
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C56" s="5"/>
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C57" s="5"/>
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C58" s="5"/>
+      <c r="D58" s="4"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C59" s="5"/>
+      <c r="D59" s="4"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C60" s="5"/>
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C61" s="5"/>
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C62" s="5"/>
+      <c r="D62" s="4"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C63" s="5"/>
+      <c r="D63" s="4"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C64" s="5"/>
+      <c r="D64" s="4"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C65" s="5"/>
+      <c r="D65" s="4"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C66" s="5"/>
+      <c r="D66" s="4"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C67" s="5"/>
+      <c r="D67" s="4"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C68" s="5"/>
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C69" s="5"/>
+      <c r="D69" s="4"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C70" s="5"/>
+      <c r="D70" s="4"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C71" s="5"/>
+      <c r="D71" s="4"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C72" s="5"/>
+      <c r="D72" s="4"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C73" s="5"/>
+      <c r="D73" s="4"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C74" s="5"/>
+      <c r="D74" s="4"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C75" s="5"/>
+      <c r="D75" s="4"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C76" s="5"/>
+      <c r="D76" s="4"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C77" s="5"/>
+      <c r="D77" s="4"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C78" s="5"/>
+      <c r="D78" s="4"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C79" s="5"/>
+      <c r="D79" s="4"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C80" s="5"/>
+      <c r="D80" s="4"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C81" s="5"/>
+      <c r="D81" s="4"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C82" s="5"/>
+      <c r="D82" s="4"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C83" s="5"/>
+      <c r="D83" s="4"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C84" s="5"/>
+      <c r="D84" s="4"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C85" s="5"/>
+      <c r="D85" s="4"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C86" s="5"/>
+      <c r="D86" s="4"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C87" s="5"/>
+      <c r="D87" s="4"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C88" s="5"/>
+      <c r="D88" s="4"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C89" s="5"/>
+      <c r="D89" s="4"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C90" s="5"/>
+      <c r="D90" s="4"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C91" s="5"/>
+      <c r="D91" s="4"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C92" s="5"/>
+      <c r="D92" s="4"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C93" s="5"/>
+      <c r="D93" s="4"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C94" s="5"/>
+      <c r="D94" s="4"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C95" s="5"/>
+      <c r="D95" s="4"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C96" s="5"/>
+      <c r="D96" s="4"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C97" s="5"/>
+      <c r="D97" s="4"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C98" s="5"/>
+      <c r="D98" s="4"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C99" s="5"/>
+      <c r="D99" s="4"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C100" s="5"/>
+      <c r="D100" s="4"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C101" s="5"/>
+      <c r="D101" s="4"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C102" s="5"/>
+      <c r="D102" s="4"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C103" s="5"/>
+      <c r="D103" s="4"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C104" s="5"/>
+      <c r="D104" s="4"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C105" s="5"/>
+      <c r="D105" s="4"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C106" s="5"/>
+      <c r="D106" s="4"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C107" s="5"/>
+      <c r="D107" s="4"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C108" s="5"/>
+      <c r="D108" s="4"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C109" s="5"/>
+      <c r="D109" s="4"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C110" s="5"/>
+      <c r="D110" s="4"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C111" s="5"/>
+      <c r="D111" s="4"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C112" s="5"/>
+      <c r="D112" s="4"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C113" s="5"/>
+      <c r="D113" s="4"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C114" s="5"/>
+      <c r="D114" s="4"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C115" s="5"/>
+      <c r="D115" s="4"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C116" s="5"/>
+      <c r="D116" s="4"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C117" s="5"/>
+      <c r="D117" s="4"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C118" s="5"/>
+      <c r="D118" s="4"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C119" s="5"/>
+      <c r="D119" s="4"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C120" s="5"/>
+      <c r="D120" s="4"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C121" s="5"/>
+      <c r="D121" s="4"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C122" s="5"/>
+      <c r="D122" s="4"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C123" s="5"/>
+      <c r="D123" s="4"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C124" s="5"/>
+      <c r="D124" s="4"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C125" s="5"/>
+      <c r="D125" s="4"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C126" s="5"/>
+      <c r="D126" s="4"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C127" s="5"/>
+      <c r="D127" s="4"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C128" s="5"/>
+      <c r="D128" s="4"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C129" s="5"/>
+      <c r="D129" s="4"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C130" s="5"/>
+      <c r="D130" s="4"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C131" s="5"/>
+      <c r="D131" s="4"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C132" s="5"/>
+      <c r="D132" s="4"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C133" s="5"/>
+      <c r="D133" s="4"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C134" s="5"/>
+      <c r="D134" s="4"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C135" s="5"/>
+      <c r="D135" s="4"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C136" s="5"/>
+      <c r="D136" s="4"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C137" s="5"/>
+      <c r="D137" s="4"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C138" s="5"/>
+      <c r="D138" s="4"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C139" s="5"/>
+      <c r="D139" s="4"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C140" s="5"/>
+      <c r="D140" s="4"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C141" s="5"/>
+      <c r="D141" s="4"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C142" s="5"/>
+      <c r="D142" s="4"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C143" s="5"/>
+      <c r="D143" s="4"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>141</v>
       </c>
@@ -3499,5 +4958,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>